<commit_message>
final pdf and code
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Downloads\Assignments\NN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Downloads\Assignments\NN\NN_CS6673\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1D7248-FA0D-4C1C-9CA7-1C04BF7D109E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C681EC-E9A8-4D6E-9BAD-7BA5D38DAB8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1455" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26760" yWindow="4155" windowWidth="16920" windowHeight="10545" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XOR weights validation" sheetId="1" r:id="rId1"/>
@@ -19229,8 +19229,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P601"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M502" sqref="M502:P502"/>
+    <sheetView topLeftCell="A601" workbookViewId="0">
+      <selection activeCell="D502" sqref="D502:D601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35689,7 +35689,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="512" spans="1:16" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="512" spans="1:16" ht="304.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A512" s="3" t="s">
         <v>74</v>
       </c>
@@ -38574,6 +38574,11 @@
     <filterColumn colId="0">
       <filters>
         <filter val="[ 2, 10, 1]"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="Yes"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -39495,8 +39500,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P601"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R502" sqref="R502"/>
+    <sheetView tabSelected="1" topLeftCell="A601" workbookViewId="0">
+      <selection activeCell="D502" sqref="D502:D601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -58855,7 +58860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97D89B0-D679-4A85-ACA9-40692D15A65D}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>

</xml_diff>